<commit_message>
Ausimplementierung Produktvorschlag + Update Embedding
</commit_message>
<xml_diff>
--- a/produkteinstufung/ProduktMetadaten.xlsx
+++ b/produkteinstufung/ProduktMetadaten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\AnlageberaterGPT\Testdaten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\AnlageberaterGPT\produkteinstufung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32788F0F-66C8-4BAB-91D2-61771C494FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05BC873-FF6A-4924-ADB4-297E507986D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Produktname</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Festgeld</t>
   </si>
   <si>
-    <t>3 Monate</t>
-  </si>
-  <si>
-    <t>Kein Risiko</t>
-  </si>
-  <si>
     <t>Nach 3 Monaten</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Sparbrief</t>
   </si>
   <si>
-    <t>Ab 1 Jahr</t>
-  </si>
-  <si>
     <t>Jährlich zum Kalenderjahresende</t>
   </si>
   <si>
@@ -87,13 +78,16 @@
     <t>Tagesgeld</t>
   </si>
   <si>
-    <t>unbefristet</t>
-  </si>
-  <si>
     <t>jeweils zum Quartalsschluss</t>
   </si>
   <si>
-    <t>Kein Mindestanlagebetrag</t>
+    <t>mittelfristig</t>
+  </si>
+  <si>
+    <t>kurzfristig</t>
+  </si>
+  <si>
+    <t>kein Risiko</t>
   </si>
 </sst>
 </file>
@@ -414,7 +408,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +446,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -469,24 +463,24 @@
         <v>5000</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>20240102</v>
@@ -495,42 +489,42 @@
         <v>1000</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>20230401</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimize filter and update database with new Products
</commit_message>
<xml_diff>
--- a/produkteinstufung/ProduktMetadaten.xlsx
+++ b/produkteinstufung/ProduktMetadaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\AnlageberaterGPT\produkteinstufung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05BC873-FF6A-4924-ADB4-297E507986D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DC5D58B-0A03-4BD7-827D-D381B549434B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2136" yWindow="1152" windowWidth="17256" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Produktname</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Laufzeit</t>
   </si>
   <si>
-    <t>Gutschrift</t>
-  </si>
-  <si>
     <t>Dateiname</t>
   </si>
   <si>
@@ -54,33 +51,21 @@
     <t>Festgeld</t>
   </si>
   <si>
-    <t>Nach 3 Monaten</t>
-  </si>
-  <si>
     <t>Kosten</t>
   </si>
   <si>
-    <t>Kostenfrei</t>
-  </si>
-  <si>
     <t>PIB_VReG-Sparbrief_20240102.pdf</t>
   </si>
   <si>
     <t>Sparbrief</t>
   </si>
   <si>
-    <t>Jährlich zum Kalenderjahresende</t>
-  </si>
-  <si>
     <t>VReG_Tagesgeld_20230401.pdf</t>
   </si>
   <si>
     <t>Tagesgeld</t>
   </si>
   <si>
-    <t>jeweils zum Quartalsschluss</t>
-  </si>
-  <si>
     <t>mittelfristig</t>
   </si>
   <si>
@@ -88,6 +73,36 @@
   </si>
   <si>
     <t>kein Risiko</t>
+  </si>
+  <si>
+    <t>Aktienfond</t>
+  </si>
+  <si>
+    <t>Bonuszertifikat</t>
+  </si>
+  <si>
+    <t>PIB_Union_Aktienfond_9766865.pdf</t>
+  </si>
+  <si>
+    <t>PIB_DZBank_Bonuszertifikat_7035880.pdf</t>
+  </si>
+  <si>
+    <t>langfristig</t>
+  </si>
+  <si>
+    <t>mittleres Risiko</t>
+  </si>
+  <si>
+    <t>hohes Risiko</t>
+  </si>
+  <si>
+    <t>Nachhaltigkeit</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -405,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,7 +440,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -443,18 +458,18 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2">
         <v>10400552</v>
@@ -463,24 +478,24 @@
         <v>5000</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>20240102</v>
@@ -489,24 +504,24 @@
         <v>1000</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>20230401</v>
@@ -515,16 +530,68 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>9766865</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
-        <v>11</v>
+      <c r="C6">
+        <v>7035880</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Produktdaten und diverse Cleanups
</commit_message>
<xml_diff>
--- a/produkteinstufung/ProduktMetadaten.xlsx
+++ b/produkteinstufung/ProduktMetadaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\AnlageberaterGPT\produkteinstufung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DC5D58B-0A03-4BD7-827D-D381B549434B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CB6F98-707C-48E8-8AD1-1E574F7E49A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2136" yWindow="1152" windowWidth="17256" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Produktname</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>ja</t>
+  </si>
+  <si>
+    <t>PIB_VRWestmuensterland_MischfondNachhaltig_623669.pdf</t>
+  </si>
+  <si>
+    <t>Mischfond</t>
+  </si>
+  <si>
+    <t>PIB_Union_PrivatFond_12345678.pdf</t>
+  </si>
+  <si>
+    <t>Privatfond</t>
+  </si>
+  <si>
+    <t>PIB_UnionAsia_Aktienfond_971267.pdf</t>
   </si>
 </sst>
 </file>
@@ -420,20 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -570,13 +585,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C6">
-        <v>7035880</v>
+        <v>623669</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -585,12 +600,90 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
       </c>
       <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>12345678</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>7035880</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>971267</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>